<commit_message>
ein paar vorarbeiten für die time agreegation- umgeschrieben von exercise 3 zu raphaels time agregation jetzt also mit _long_time_storrage
</commit_message>
<xml_diff>
--- a/Time Aggregation/modified_time_series_data.xlsx
+++ b/Time Aggregation/modified_time_series_data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eva-m\Documents\Uni\SS2024\ModE\Projekt\Sourcetree_Daten\Time Aggregation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0869F71F-A4FE-4F15-B24F-E18B362FBA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -37,8 +43,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,17 +103,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -145,7 +159,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -179,6 +193,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -213,9 +228,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -388,14 +404,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,7 +433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -429,13 +447,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>141.020666839994</v>
+        <v>141.02066683999399</v>
       </c>
       <c r="F2">
-        <v>0.2113521774595594</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.21135217745955939</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -443,19 +461,19 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>179.6651416329921</v>
+        <v>179.66514163299209</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>145.882326994503</v>
+        <v>145.88232699450299</v>
       </c>
       <c r="F3">
         <v>0.2095531652758385</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -463,19 +481,19 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>172.0037715335249</v>
+        <v>172.00377153352491</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>143.1042354776407</v>
+        <v>143.10423547764071</v>
       </c>
       <c r="F4">
-        <v>0.20995857647217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>0.20995857647217001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -483,19 +501,19 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>161.556448582926</v>
+        <v>161.55644858292601</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>142.4097125984252</v>
+        <v>142.40971259842519</v>
       </c>
       <c r="F5">
-        <v>0.2120869852529098</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0.21208698525290981</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -503,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>157.3775194268009</v>
+        <v>157.37751942680089</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -515,7 +533,7 @@
         <v>0.2327376180660424</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
@@ -523,19 +541,19 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>149.0196611145508</v>
+        <v>149.01966111455079</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>147.9658956321497</v>
+        <v>147.96589563214971</v>
       </c>
       <c r="F7">
-        <v>0.2783463776533285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0.27834637765332848</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -543,19 +561,19 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>144.4924878520343</v>
+        <v>144.49248785203429</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>150.0494642697965</v>
+        <v>150.04946426979649</v>
       </c>
       <c r="F8">
-        <v>0.3113113755550281</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0.31131137555502808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -569,13 +587,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>184.775608230575</v>
+        <v>184.77560823057499</v>
       </c>
       <c r="F9">
-        <v>0.3315312589720582</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0.33153125897205821</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -586,16 +604,16 @@
         <v>134.0451649014353</v>
       </c>
       <c r="D10">
-        <v>3.091940006180882</v>
+        <v>3.0919400061808822</v>
       </c>
       <c r="E10">
-        <v>212.5565233991977</v>
+        <v>212.55652339919769</v>
       </c>
       <c r="F10">
         <v>0.2689965819379348</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -609,13 +627,13 @@
         <v>100.3034987493858</v>
       </c>
       <c r="E11">
-        <v>227.8360267419403</v>
+        <v>227.83602674194029</v>
       </c>
       <c r="F11">
         <v>0.2393508882061989</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -626,16 +644,16 @@
         <v>135.7863854333927</v>
       </c>
       <c r="D12">
-        <v>234.2571282544056</v>
+        <v>234.25712825440559</v>
       </c>
       <c r="E12">
-        <v>226.4469809835091</v>
+        <v>226.44698098350909</v>
       </c>
       <c r="F12">
         <v>0.2289115499006647</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
@@ -643,19 +661,19 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>145.1889760648172</v>
+        <v>145.18897606481721</v>
       </c>
       <c r="D13">
-        <v>345.3733208205991</v>
+        <v>345.37332082059908</v>
       </c>
       <c r="E13">
-        <v>225.057935225078</v>
+        <v>225.05793522507801</v>
       </c>
       <c r="F13">
-        <v>0.1932860410230398</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>0.19328604102303981</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
@@ -663,19 +681,19 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>153.1985902706759</v>
+        <v>153.19859027067591</v>
       </c>
       <c r="D14">
-        <v>398.736183324071</v>
+        <v>398.73618332407102</v>
       </c>
       <c r="E14">
-        <v>222.9743665874313</v>
+        <v>222.97436658743129</v>
       </c>
       <c r="F14">
         <v>0.1761827561778071</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0</v>
       </c>
@@ -683,19 +701,19 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>138.2240940575604</v>
+        <v>138.22409405756039</v>
       </c>
       <c r="D15">
-        <v>383.4979917205735</v>
+        <v>383.49799172057351</v>
       </c>
       <c r="E15">
-        <v>238.9483928093894</v>
+        <v>238.94839280938939</v>
       </c>
       <c r="F15">
-        <v>0.1667569458631016</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>0.16675694586310161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
@@ -703,10 +721,10 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>138.2240940575604</v>
+        <v>138.22409405756039</v>
       </c>
       <c r="D16">
-        <v>286.7395619563825</v>
+        <v>286.73956195638249</v>
       </c>
       <c r="E16">
         <v>254.2278961521319</v>
@@ -715,7 +733,7 @@
         <v>0.1742063765956916</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0</v>
       </c>
@@ -726,16 +744,16 @@
         <v>121.1601333266687</v>
       </c>
       <c r="D17">
-        <v>74.89577011973689</v>
+        <v>74.895770119736895</v>
       </c>
       <c r="E17">
-        <v>214.6400920368445</v>
+        <v>214.64009203684449</v>
       </c>
       <c r="F17">
-        <v>0.1870021674799024</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>0.18700216747990239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0</v>
       </c>
@@ -743,19 +761,19 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>130.5627239580932</v>
+        <v>130.56272395809319</v>
       </c>
       <c r="D18">
         <v>25.08442208327158</v>
       </c>
       <c r="E18">
-        <v>202.8332030901798</v>
+        <v>202.83320309017981</v>
       </c>
       <c r="F18">
-        <v>0.2201191945802264</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>0.22011919458022641</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0</v>
       </c>
@@ -763,19 +781,19 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>119.070668784778</v>
+        <v>119.07066878477799</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>171.5796735254791</v>
+        <v>171.57967352547911</v>
       </c>
       <c r="F19">
-        <v>0.2555166596599144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>0.25551665965991438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0</v>
       </c>
@@ -795,7 +813,7 @@
         <v>0.291598256133412</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0</v>
       </c>
@@ -809,13 +827,13 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>139.6316210815629</v>
+        <v>139.63162108156291</v>
       </c>
       <c r="F21">
-        <v>0.2985915992701293</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>0.29859159927012929</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0</v>
       </c>
@@ -823,19 +841,19 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>117.3294483010497</v>
+        <v>117.32944830104969</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>136.1590066854851</v>
+        <v>136.15900668548511</v>
       </c>
       <c r="F22">
-        <v>0.2808801976304001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>0.28088019763040012</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0</v>
       </c>
@@ -849,13 +867,13 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>137.5480524439162</v>
+        <v>137.54805244391619</v>
       </c>
       <c r="F23">
-        <v>0.2382866838158288</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>0.23828668381582879</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0</v>
       </c>
@@ -863,19 +881,19 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>166.0836218454425</v>
+        <v>166.08362184544251</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>129.2137778933294</v>
+        <v>129.21377789332939</v>
       </c>
       <c r="F24">
-        <v>0.2297730486928689</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>0.22977304869286891</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0</v>
       </c>
@@ -883,44 +901,44 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>188.7194881580251</v>
+        <v>188.71948815802509</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>128.5192550141138</v>
+        <v>128.51925501411381</v>
       </c>
       <c r="F25">
-        <v>0.2477378323303051</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>0.24773783233030511</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <v>115.985593061626</v>
+        <v>115.98559306162601</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>150.0494642697965</v>
+        <v>150.04946426979649</v>
       </c>
       <c r="F26">
-        <v>0.1844683475028311</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>0.18446834750283109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C27">
         <v>114.2968826527444</v>
@@ -929,18 +947,18 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>139.6316210815629</v>
+        <v>139.63162108156291</v>
       </c>
       <c r="F27">
-        <v>0.1530743179869156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>0.15307431798691559</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C28">
         <v>108.386396203573</v>
@@ -949,21 +967,21 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>138.9370982023474</v>
+        <v>138.93709820234741</v>
       </c>
       <c r="F28">
-        <v>0.1483614128295629</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>0.14836141282956289</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C29">
-        <v>92.85026040810209</v>
+        <v>92.850260408102088</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -972,38 +990,38 @@
         <v>140.3261439607785</v>
       </c>
       <c r="F29">
-        <v>0.1512246294036536</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>0.15122462940365361</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>88.79735540749466</v>
+        <v>88.797355407494663</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>152.1330329074432</v>
+        <v>152.13303290744321</v>
       </c>
       <c r="F30">
         <v>0.1278374710152741</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C31">
-        <v>77.82073773167849</v>
+        <v>77.820737731678491</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1012,35 +1030,35 @@
         <v>167.4125362501857</v>
       </c>
       <c r="F31">
-        <v>0.1718499240170152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>0.17184992401701521</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C32">
-        <v>84.91332145862695</v>
+        <v>84.913321458626953</v>
       </c>
       <c r="D32">
-        <v>2.475055973680672</v>
+        <v>2.4750559736806719</v>
       </c>
       <c r="E32">
-        <v>241.7264843262517</v>
+        <v>241.72648432625169</v>
       </c>
       <c r="F32">
-        <v>0.2251108199350572</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>0.22511081993505719</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C33">
         <v>74.44331690185804</v>
@@ -1049,161 +1067,161 @@
         <v>120.5194996100258</v>
       </c>
       <c r="E33">
-        <v>266.0347850987966</v>
+        <v>266.03478509879659</v>
       </c>
       <c r="F33">
-        <v>0.2676029809505456</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>0.26760298095054558</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C34">
-        <v>64.31105442445403</v>
+        <v>64.311054424454028</v>
       </c>
       <c r="D34">
-        <v>190.2097633567058</v>
+        <v>190.20976335670579</v>
       </c>
       <c r="E34">
-        <v>220.196275070569</v>
+        <v>220.19627507056899</v>
       </c>
       <c r="F34">
-        <v>0.2878482025673464</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>0.28784820256734639</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C35">
-        <v>62.28460192415032</v>
+        <v>62.284601924150323</v>
       </c>
       <c r="D35">
-        <v>438.1733238004331</v>
+        <v>438.17332380043308</v>
       </c>
       <c r="E35">
-        <v>225.7524581042936</v>
+        <v>225.75245810429359</v>
       </c>
       <c r="F35">
-        <v>0.2639036037840209</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>0.26390360378402089</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C36">
-        <v>59.24492318575202</v>
+        <v>59.244923185752022</v>
       </c>
       <c r="D36">
         <v>442.2041466375826</v>
       </c>
       <c r="E36">
-        <v>226.4469809835091</v>
+        <v>226.44698098350909</v>
       </c>
       <c r="F36">
-        <v>0.2480418907275538</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>0.24804189072755381</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C37">
-        <v>62.62234400351517</v>
+        <v>62.622344003515167</v>
       </c>
       <c r="D37">
-        <v>516.9051480493141</v>
+        <v>516.90514804931411</v>
       </c>
       <c r="E37">
-        <v>238.9483928093894</v>
+        <v>238.94839280938939</v>
       </c>
       <c r="F37">
-        <v>0.2389708152096378</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>0.23897081520963781</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C38">
         <v>59.41379422543443</v>
       </c>
       <c r="D38">
-        <v>592.7458028115489</v>
+        <v>592.74580281154886</v>
       </c>
       <c r="E38">
-        <v>213.9455691576289</v>
+        <v>213.94556915762891</v>
       </c>
       <c r="F38">
-        <v>0.2336244550580175</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>0.23362445505801749</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C39">
-        <v>62.62234400351517</v>
+        <v>62.622344003515167</v>
       </c>
       <c r="D39">
-        <v>488.5586086342561</v>
+        <v>488.55860863425607</v>
       </c>
       <c r="E39">
-        <v>198.6660658148863</v>
+        <v>198.66606581488631</v>
       </c>
       <c r="F39">
-        <v>0.2315720608765895</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>0.23157206087658949</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C40">
-        <v>54.85427610577971</v>
+        <v>54.854276105779711</v>
       </c>
       <c r="D40">
-        <v>420.0743222323304</v>
+        <v>420.07432223233042</v>
       </c>
       <c r="E40">
-        <v>190.3317912642995</v>
+        <v>190.33179126429951</v>
       </c>
       <c r="F40">
         <v>0.2250854817352865</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C41">
-        <v>55.36088923688428</v>
+        <v>55.360889236884283</v>
       </c>
       <c r="D41">
         <v>219.6027753162486</v>
@@ -1215,195 +1233,195 @@
         <v>0.2316480754759016</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C42">
         <v>45.90411091820998</v>
       </c>
       <c r="D42">
-        <v>114.7864365345582</v>
+        <v>114.78643653455821</v>
       </c>
       <c r="E42">
-        <v>153.5220786658743</v>
+        <v>153.52207866587429</v>
       </c>
       <c r="F42">
         <v>0.2421127519812068</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C43">
-        <v>46.5795950769397</v>
+        <v>46.579595076939697</v>
       </c>
       <c r="D43">
-        <v>17.22870811871613</v>
+        <v>17.228708118716131</v>
       </c>
       <c r="E43">
-        <v>141.020666839994</v>
+        <v>141.02066683999399</v>
       </c>
       <c r="F43">
-        <v>0.2584052144337761</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>0.25840521443377612</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C44">
-        <v>44.72201362837568</v>
+        <v>44.722013628375677</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>143.1042354776407</v>
+        <v>143.10423547764071</v>
       </c>
       <c r="F44">
-        <v>0.2646384115773719</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>0.26463841157737189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C45">
-        <v>56.37411547497886</v>
+        <v>56.374115474978858</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>144.4932812360719</v>
+        <v>144.49328123607191</v>
       </c>
       <c r="F45">
         <v>0.2375265378227075</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C46">
-        <v>50.80137111722956</v>
+        <v>50.801371117229557</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>141.020666839994</v>
+        <v>141.02066683999399</v>
       </c>
       <c r="F46">
-        <v>0.2293422992967666</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>0.22934229929676661</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C47">
-        <v>54.17879194705001</v>
+        <v>54.178791947050009</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>138.9370982023474</v>
+        <v>138.93709820234741</v>
       </c>
       <c r="F47">
-        <v>0.2219942213632592</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>0.22199422136325919</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1</v>
       </c>
       <c r="B48">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C48">
-        <v>73.09234857234134</v>
+        <v>73.092348572341336</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>139.6316210815629</v>
+        <v>139.63162108156291</v>
       </c>
       <c r="F48">
-        <v>0.200887500954254</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>0.20088750095425401</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1</v>
       </c>
       <c r="B49">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C49">
-        <v>77.98960877136092</v>
+        <v>77.989608771360921</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>125.7411634972515</v>
+        <v>125.74116349725151</v>
       </c>
       <c r="F49">
-        <v>0.1810476905337844</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>0.18104769053378439</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C50">
-        <v>72.76691185356246</v>
+        <v>72.766911853562462</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>134.7699609270539</v>
+        <v>134.76996092705389</v>
       </c>
       <c r="F50">
         <v>0.1286482934079369</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C51">
-        <v>59.40512220264886</v>
+        <v>59.405122202648862</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1412,38 +1430,38 @@
         <v>131.9918694101917</v>
       </c>
       <c r="F51">
-        <v>0.1128372567510108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>0.11283725675101081</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C52">
-        <v>47.60510016168312</v>
+        <v>47.605100161683119</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>131.2973465309761</v>
+        <v>131.29734653097611</v>
       </c>
       <c r="F52">
-        <v>0.1160298699221212</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>0.11602986992212121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C53">
-        <v>41.1844999338652</v>
+        <v>41.184499933865197</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1452,175 +1470,175 @@
         <v>134.0754380478383</v>
       </c>
       <c r="F53">
-        <v>0.09363090132480936</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>9.3630901324809362E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C54">
-        <v>42.65950269200024</v>
+        <v>42.659502692000238</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>142.4097125984252</v>
+        <v>142.40971259842519</v>
       </c>
       <c r="F54">
         <v>0.1088084829874673</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C55">
-        <v>41.96538374486775</v>
+        <v>41.965383744867751</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>150.0494642697965</v>
+        <v>150.04946426979649</v>
       </c>
       <c r="F55">
         <v>0.1585727073371607</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C56">
-        <v>43.70068110667032</v>
+        <v>43.700681106670316</v>
       </c>
       <c r="D56">
-        <v>68.36572042212703</v>
+        <v>68.365720422127026</v>
       </c>
       <c r="E56">
-        <v>166.7180133709701</v>
+        <v>166.71801337097011</v>
       </c>
       <c r="F56">
         <v>0.2481685817264076</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2</v>
       </c>
       <c r="B57">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="C57">
-        <v>37.62714034639001</v>
+        <v>37.627140346390007</v>
       </c>
       <c r="D57">
-        <v>255.9264204599236</v>
+        <v>255.92642045992361</v>
       </c>
       <c r="E57">
-        <v>176.4413336799881</v>
+        <v>176.44133367998811</v>
       </c>
       <c r="F57">
-        <v>0.3382712201110685</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>0.33827122011106853</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2</v>
       </c>
       <c r="B58">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C58">
-        <v>35.54478351704984</v>
+        <v>35.544783517049837</v>
       </c>
       <c r="D58">
-        <v>489.3596354579747</v>
+        <v>489.35963545797472</v>
       </c>
       <c r="E58">
-        <v>196.5824971772396</v>
+        <v>196.58249717723959</v>
       </c>
       <c r="F58">
-        <v>0.3518018187886303</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>0.35180181878863032</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2</v>
       </c>
       <c r="B59">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C59">
-        <v>29.21094816515929</v>
+        <v>29.210948165159291</v>
       </c>
       <c r="D59">
-        <v>698.7055314604208</v>
+        <v>698.70553146042084</v>
       </c>
       <c r="E59">
-        <v>191.0263141435151</v>
+        <v>191.02631414351509</v>
       </c>
       <c r="F59">
-        <v>0.3545130061640964</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>0.35451300616409642</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
       <c r="B60">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C60">
-        <v>28.60359409395416</v>
+        <v>28.603594093954161</v>
       </c>
       <c r="D60">
-        <v>863.4694999377726</v>
+        <v>863.46949993777264</v>
       </c>
       <c r="E60">
         <v>200.0551115733175</v>
       </c>
       <c r="F60">
-        <v>0.3508643053971137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>0.35086430539711372</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2</v>
       </c>
       <c r="B61">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C61">
         <v>32.50801314896696</v>
       </c>
       <c r="D61">
-        <v>986.2274373068275</v>
+        <v>986.22743730682748</v>
       </c>
       <c r="E61">
-        <v>209.0839090031199</v>
+        <v>209.08390900311991</v>
       </c>
       <c r="F61">
         <v>0.345137872248932</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2</v>
       </c>
       <c r="B62">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C62">
         <v>28.2565346143593</v>
@@ -1629,84 +1647,84 @@
         <v>1025.1507997689</v>
       </c>
       <c r="E62">
-        <v>225.057935225078</v>
+        <v>225.05793522507801</v>
       </c>
       <c r="F62">
-        <v>0.3477477068253157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>0.34774770682531569</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2</v>
       </c>
       <c r="B63">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C63">
-        <v>27.90947514682168</v>
+        <v>27.909475146821681</v>
       </c>
       <c r="D63">
-        <v>994.230699058544</v>
+        <v>994.23069905854402</v>
       </c>
       <c r="E63">
-        <v>229.919595379587</v>
+        <v>229.91959537958701</v>
       </c>
       <c r="F63">
-        <v>0.3461767384395313</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>0.34617673843953128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2</v>
       </c>
       <c r="B64">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="C64">
         <v>29.81830223636441</v>
       </c>
       <c r="D64">
-        <v>906.1574546228808</v>
+        <v>906.15745462288078</v>
       </c>
       <c r="E64">
-        <v>215.33461491606</v>
+        <v>215.33461491605999</v>
       </c>
       <c r="F64">
-        <v>0.3574268991377286</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>0.35742689913772863</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>2</v>
       </c>
       <c r="B65">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C65">
-        <v>27.12859133581913</v>
+        <v>27.128591335819131</v>
       </c>
       <c r="D65">
-        <v>747.4677445916129</v>
+        <v>747.46774459161293</v>
       </c>
       <c r="E65">
-        <v>213.9455691576289</v>
+        <v>213.94556915762891</v>
       </c>
       <c r="F65">
-        <v>0.3755183737740189</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>0.37551837377401892</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>2</v>
       </c>
       <c r="B66">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C66">
-        <v>25.91388318135161</v>
+        <v>25.913883181351611</v>
       </c>
       <c r="D66">
-        <v>551.7906816091316</v>
+        <v>551.79068160913164</v>
       </c>
       <c r="E66">
         <v>186.1646539890061</v>
@@ -1715,72 +1733,72 @@
         <v>0.3946487146009085</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2</v>
       </c>
       <c r="B67">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C67">
-        <v>25.39329397401657</v>
+        <v>25.393293974016569</v>
       </c>
       <c r="D67">
-        <v>325.6045403557508</v>
+        <v>325.60454035575083</v>
       </c>
       <c r="E67">
         <v>162.5508760956767</v>
       </c>
       <c r="F67">
-        <v>0.4126641746378865</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>0.41266417463788652</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>2</v>
       </c>
       <c r="B68">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="C68">
-        <v>24.52564529914393</v>
+        <v>24.525645299143932</v>
       </c>
       <c r="D68">
         <v>115.6309009198917</v>
       </c>
       <c r="E68">
-        <v>152.8275557866587</v>
+        <v>152.82755578665871</v>
       </c>
       <c r="F68">
-        <v>0.4246744813292053</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+        <v>0.42467448132920532</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>2</v>
       </c>
       <c r="B69">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="C69">
-        <v>29.03741842536185</v>
+        <v>29.037418425361849</v>
       </c>
       <c r="D69">
-        <v>4.113144055893892</v>
+        <v>4.1131440558938923</v>
       </c>
       <c r="E69">
-        <v>138.9370982023474</v>
+        <v>138.93709820234741</v>
       </c>
       <c r="F69">
-        <v>0.3986268119649107</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <v>0.39862681196491068</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>2</v>
       </c>
       <c r="B70">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C70">
         <v>27.04182647194904</v>
@@ -1789,18 +1807,18 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <v>133.3809151686228</v>
+        <v>133.38091516862281</v>
       </c>
       <c r="F70">
-        <v>0.3695892350276715</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>0.36958923502767149</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>2</v>
       </c>
       <c r="B71">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C71">
         <v>26.86829673215161</v>
@@ -1809,21 +1827,21 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>134.7699609270539</v>
+        <v>134.76996092705389</v>
       </c>
       <c r="F71">
-        <v>0.3408810546874522</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+        <v>0.34088105468745222</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>2</v>
       </c>
       <c r="B72">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="C72">
-        <v>37.10655113905496</v>
+        <v>37.106551139054957</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -1832,38 +1850,38 @@
         <v>138.2425753231318</v>
       </c>
       <c r="F72">
-        <v>0.3237524316424488</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+        <v>0.32375243164244882</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>2</v>
       </c>
       <c r="B73">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C73">
-        <v>45.34921359254552</v>
+        <v>45.349213592545517</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>137.5480524439162</v>
+        <v>137.54805244391619</v>
       </c>
       <c r="F73">
-        <v>0.2966658960875552</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+        <v>0.29666589608755523</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>3</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="C74">
-        <v>319.1228532532223</v>
+        <v>319.12285325322227</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -1872,38 +1890,38 @@
         <v>112.5452287921557</v>
       </c>
       <c r="F74">
-        <v>0.2036747029290326</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <v>0.20367470292903261</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>3</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="C75">
-        <v>328.526953937166</v>
+        <v>328.52695393716601</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>113.2397516713713</v>
+        <v>113.23975167137129</v>
       </c>
       <c r="F75">
         <v>0.1962759485959843</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>3</v>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="C76">
-        <v>316.7718280822364</v>
+        <v>316.77182808223642</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -1915,12 +1933,12 @@
         <v>0.1951864060058433</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>3</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="C77">
         <v>302.6656771768935</v>
@@ -1932,18 +1950,18 @@
         <v>116.0178431882336</v>
       </c>
       <c r="F77">
-        <v>0.1979229315810805</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+        <v>0.19792293158108051</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>3</v>
       </c>
       <c r="B78">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="C78">
-        <v>283.269719576546</v>
+        <v>283.26971957654598</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -1955,15 +1973,15 @@
         <v>0.2161664354159947</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>3</v>
       </c>
       <c r="B79">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="C79">
-        <v>273.8656188926024</v>
+        <v>273.86561889260241</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -1972,38 +1990,38 @@
         <v>120.8795033427425</v>
       </c>
       <c r="F79">
-        <v>0.2646384115773719</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+        <v>0.26463841157737189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>3</v>
       </c>
       <c r="B80">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="C80">
-        <v>260.9349805727525</v>
+        <v>260.93498057275252</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="E80">
-        <v>132.6863922894072</v>
+        <v>132.68639228940719</v>
       </c>
       <c r="F80">
         <v>0.288506995761385</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>3</v>
       </c>
       <c r="B81">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="C81">
-        <v>260.9349805727525</v>
+        <v>260.93498057275252</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2012,58 +2030,58 @@
         <v>165.328967612539</v>
       </c>
       <c r="F81">
-        <v>0.2806014774329221</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>0.28060147743292208</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>3</v>
       </c>
       <c r="B82">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="C82">
-        <v>252.118636121269</v>
+        <v>252.11863612126899</v>
       </c>
       <c r="D82">
-        <v>4.10032295675164</v>
+        <v>4.1003229567516399</v>
       </c>
       <c r="E82">
-        <v>185.4701311097905</v>
+        <v>185.47013110979049</v>
       </c>
       <c r="F82">
-        <v>0.2478645233291586</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>0.24786452332915859</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>3</v>
       </c>
       <c r="B83">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C83">
-        <v>248.00434213233</v>
+        <v>248.00434213233001</v>
       </c>
       <c r="D83">
         <v>48.56277381587217</v>
       </c>
       <c r="E83">
-        <v>193.1098827811618</v>
+        <v>193.10988278116179</v>
       </c>
       <c r="F83">
-        <v>0.2070193452987669</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+        <v>0.20701934529876689</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>3</v>
       </c>
       <c r="B84">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="C84">
-        <v>233.3104348739543</v>
+        <v>233.31043487395431</v>
       </c>
       <c r="D84">
         <v>109.5279176068771</v>
@@ -2072,115 +2090,115 @@
         <v>193.8044056603774</v>
       </c>
       <c r="F84">
-        <v>0.1616893059089587</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+        <v>0.16168930590895869</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>3</v>
       </c>
       <c r="B85">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="C85">
-        <v>235.0737038124801</v>
+        <v>235.07370381248009</v>
       </c>
       <c r="D85">
-        <v>216.6585933170146</v>
+        <v>216.65859331701461</v>
       </c>
       <c r="E85">
-        <v>191.7208370227307</v>
+        <v>191.72083702273071</v>
       </c>
       <c r="F85">
         <v>0.1485387802279575</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>3</v>
       </c>
       <c r="B86">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C86">
         <v>222.7308216045177</v>
       </c>
       <c r="D86">
-        <v>115.7985794160768</v>
+        <v>115.79857941607681</v>
       </c>
       <c r="E86">
-        <v>188.2482226266528</v>
+        <v>188.24822262665279</v>
       </c>
       <c r="F86">
-        <v>0.1387835733162326</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>0.13878357331623259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>3</v>
       </c>
       <c r="B87">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="C87">
         <v>218.6165276155786</v>
       </c>
       <c r="D87">
-        <v>69.001567546853</v>
+        <v>69.001567546852996</v>
       </c>
       <c r="E87">
-        <v>197.2770200564553</v>
+        <v>197.27702005645531</v>
       </c>
       <c r="F87">
         <v>0.1549493447699484</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>3</v>
       </c>
       <c r="B88">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="C88">
         <v>215.0899898590998</v>
       </c>
       <c r="D88">
-        <v>65.39741411663782</v>
+        <v>65.397414116637819</v>
       </c>
       <c r="E88">
-        <v>194.498928539593</v>
+        <v>194.49892853959301</v>
       </c>
       <c r="F88">
-        <v>0.1866474326831123</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+        <v>0.18664743268311229</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>3</v>
       </c>
       <c r="B89">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="C89">
         <v>192.7552508553062</v>
       </c>
       <c r="D89">
-        <v>52.99084048842985</v>
+        <v>52.990840488429853</v>
       </c>
       <c r="E89">
         <v>189.6372683850839</v>
       </c>
       <c r="F89">
-        <v>0.1958705373996525</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+        <v>0.19587053739965249</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>3</v>
       </c>
       <c r="B90">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="C90">
         <v>177.4735873644704</v>
@@ -2195,15 +2213,15 @@
         <v>0.2354488054415089</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>3</v>
       </c>
       <c r="B91">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="C91">
-        <v>184.5266627568556</v>
+        <v>184.52666275685559</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -2212,78 +2230,78 @@
         <v>154.2166015450899</v>
       </c>
       <c r="F91">
-        <v>0.2766993946682321</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+        <v>0.27669939466823212</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>3</v>
       </c>
       <c r="B92">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="C92">
-        <v>193.3430072083391</v>
+        <v>193.34300720833909</v>
       </c>
       <c r="D92">
         <v>0</v>
       </c>
       <c r="E92">
-        <v>145.882326994503</v>
+        <v>145.88232699450299</v>
       </c>
       <c r="F92">
-        <v>0.2908634483400613</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+        <v>0.29086344834006128</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>3</v>
       </c>
       <c r="B93">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="C93">
-        <v>195.1062760262922</v>
+        <v>195.10627602629219</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
       <c r="E93">
-        <v>129.2137778933294</v>
+        <v>129.21377789332939</v>
       </c>
       <c r="F93">
-        <v>0.2886336867602385</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+        <v>0.28863368676023848</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>3</v>
       </c>
       <c r="B94">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C94">
-        <v>195.6940322587523</v>
+        <v>195.69403225875229</v>
       </c>
       <c r="D94">
         <v>0</v>
       </c>
       <c r="E94">
-        <v>121.5740262219581</v>
+        <v>121.57402622195811</v>
       </c>
       <c r="F94">
-        <v>0.2630927813913582</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+        <v>0.26309278139135822</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>3</v>
       </c>
       <c r="B95">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="C95">
-        <v>227.4328719464895</v>
+        <v>227.43287194648951</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2292,18 +2310,18 @@
         <v>124.3521177388204</v>
       </c>
       <c r="F95">
-        <v>0.2471297155358083</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+        <v>0.24712971553580829</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>3</v>
       </c>
       <c r="B96">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="C96">
-        <v>269.1635685506305</v>
+        <v>269.16356855063049</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2312,27 +2330,27 @@
         <v>120.184980463527</v>
       </c>
       <c r="F96">
-        <v>0.2097812090737748</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+        <v>0.20978120907377479</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>3</v>
       </c>
       <c r="B97">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="C97">
-        <v>270.3390811361235</v>
+        <v>270.33908113612353</v>
       </c>
       <c r="D97">
         <v>0</v>
       </c>
       <c r="E97">
-        <v>118.1014118258803</v>
+        <v>118.10141182588031</v>
       </c>
       <c r="F97">
-        <v>0.222095574162342</v>
+        <v>0.22209557416234199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>